<commit_message>
add some more plots and stuff
</commit_message>
<xml_diff>
--- a/Dataset Overview.xlsx
+++ b/Dataset Overview.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\FAUbox\Semester 12\COPD_Offline_Risk_Score\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E3BE303A-B435-4699-81B6-543D9128E76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0073421-5B0C-496C-A44F-2B08162D1D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Overview" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="149">
   <si>
     <t>Exaggerate</t>
   </si>
@@ -154,9 +155,6 @@
     <t>FAMILY H/O</t>
   </si>
   <si>
-    <t>fev1</t>
-  </si>
-  <si>
     <t>FEV1</t>
   </si>
   <si>
@@ -292,9 +290,6 @@
     <t>PackHistory</t>
   </si>
   <si>
-    <t>pad</t>
-  </si>
-  <si>
     <t>PBF (Percent Body Fat)</t>
   </si>
   <si>
@@ -397,13 +392,88 @@
     <t>hospital name [hospital ]</t>
   </si>
   <si>
-    <t>Column1</t>
+    <t>Harvard</t>
+  </si>
+  <si>
+    <t>only high blood pressure</t>
+  </si>
+  <si>
+    <t>bclinpt15</t>
+  </si>
+  <si>
+    <t>bclinpt19</t>
+  </si>
+  <si>
+    <t>dem02</t>
+  </si>
+  <si>
+    <t>mmrc</t>
+  </si>
+  <si>
+    <t>can be imputed</t>
+  </si>
+  <si>
+    <t>bclinra101</t>
+  </si>
+  <si>
+    <t>dem03</t>
+  </si>
+  <si>
+    <t>bclinra11</t>
+  </si>
+  <si>
+    <t>bclinpt07</t>
+  </si>
+  <si>
+    <t>bclinpt04</t>
+  </si>
+  <si>
+    <t>socio07</t>
+  </si>
+  <si>
+    <t>bclinpt24 (needs to be binarized)</t>
+  </si>
+  <si>
+    <t>peripheral artery disease [pad]</t>
+  </si>
+  <si>
+    <t>bclinpt34 (fever), psqi11, psqi12</t>
+  </si>
+  <si>
+    <t>cant be calculated</t>
+  </si>
+  <si>
+    <t>bmi (also height bclinra01, weight bclinra02)</t>
+  </si>
+  <si>
+    <t>fev1 (not usable)</t>
+  </si>
+  <si>
+    <t>impute</t>
+  </si>
+  <si>
+    <t>could be imputed</t>
+  </si>
+  <si>
+    <t>binary could be imputed (whether standing up is at all possible)</t>
+  </si>
+  <si>
+    <t>eating might be imputed</t>
+  </si>
+  <si>
+    <t>bclinra14</t>
+  </si>
+  <si>
+    <t>bclinra01</t>
+  </si>
+  <si>
+    <t>bclinra02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -540,7 +610,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -736,6 +806,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -912,7 +988,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -924,7 +1000,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -977,6 +1056,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1001,24 +1098,6 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1033,15 +1112,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F100" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
-  <autoFilter ref="A1:F100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F100" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F100" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Exaggerate" dataDxfId="7"/>
-    <tableColumn id="2" name="GLIM" dataDxfId="6"/>
-    <tableColumn id="3" name="Kaggle" dataDxfId="5"/>
-    <tableColumn id="4" name="Palani" dataDxfId="4"/>
-    <tableColumn id="5" name="Steroid" dataDxfId="3"/>
-    <tableColumn id="6" name="Column1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Exaggerate" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="GLIM" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Kaggle" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Palani" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Steroid" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Harvard" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1343,11 +1422,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1357,7 +1436,7 @@
     <col min="3" max="3" width="18.1796875" style="1" customWidth="1"/>
     <col min="4" max="4" width="26.6328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -1375,10 +1454,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1387,6 +1466,9 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1408,7 +1490,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1427,6 +1509,9 @@
       <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
@@ -1440,7 +1525,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1468,72 +1553,90 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E18"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E19"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D25" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="F26" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
@@ -1541,17 +1644,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -1561,432 +1664,478 @@
       <c r="C31" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E32" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="D33" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="F35" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="F36" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F37" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D38" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="C39" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B44" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B46" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B48" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B50" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51"/>
+    </row>
+    <row r="52" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B52" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B59" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="C61" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B62" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B63" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B64" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B65" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B66" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B67" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C68" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B69" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B70" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B72" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B73" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B74" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B75" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C78" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B80" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B81" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="B87" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C90" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C91" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B92" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E93" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="E94" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B50" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C51" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E51"/>
-    </row>
-    <row r="52" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B52" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B53" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E56" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E57" t="s">
+      <c r="F94" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E96" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B59" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E60" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="C61" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B62" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B63" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B64" s="1" t="s">
+    <row r="97" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A97" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B98" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B99" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D100" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B65" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B66" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B67" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C68" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B69" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B70" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E71" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B72" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B73" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B74" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B75" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C78" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B80" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B81" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B82" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B87" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C90" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C91" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B92" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E93" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E94" s="1" t="s">
+      <c r="E100" s="3" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E96" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A97" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B98" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B99" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D100" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>